<commit_message>
Add AbstractSeleniumTests and initial LoginTests for three browsers. Add Seleno for self-hosting.
</commit_message>
<xml_diff>
--- a/Blog.Tests/TestData/TestData.xlsx
+++ b/Blog.Tests/TestData/TestData.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginPageModel" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,6 +21,47 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>RememberMe</t>
+  </si>
+  <si>
+    <t>ExpectedError</t>
+  </si>
+  <si>
+    <t>The Password field is required.</t>
+  </si>
+  <si>
+    <t>LoginShouldFailWithoutPassword</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>admin@admin.com</t>
+  </si>
+  <si>
+    <t>LoginShouldFailWithoutEmail</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>The Email field is required.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,12 +412,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Build and run all tests
Add new registration tests, build and run all tests, fix a spelling
error.
</commit_message>
<xml_diff>
--- a/Blog.Tests/TestData/TestData.xlsx
+++ b/Blog.Tests/TestData/TestData.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frf\Documents\Visual Studio 2015\Projects\QA-Automation-Teamwork\Blog.Tests\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageModel" sheetId="1" r:id="rId1"/>
+    <sheet name="RegistrationPageModel" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Key</t>
   </si>
@@ -60,16 +56,48 @@
   </si>
   <si>
     <t>The Email field is required.</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>NavigateToRegistrationPage</t>
+  </si>
+  <si>
+    <t>Hristina Petkova</t>
+  </si>
+  <si>
+    <t>RegisterShouldFailWithoutEmail</t>
+  </si>
+  <si>
+    <t>xrissti@gmail.com</t>
+  </si>
+  <si>
+    <t>RegisterShouldFailWithoutFullName</t>
+  </si>
+  <si>
+    <t>The Full Name field is required.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,15 +120,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Хипервръзка" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -158,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -210,7 +241,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -404,7 +435,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,4 +508,109 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>123456789</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>123456789</v>
+      </c>
+      <c r="E3">
+        <v>123456789</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>123456789</v>
+      </c>
+      <c r="E4">
+        <v>123456789</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>